<commit_message>
organizing script and excel of meta model
</commit_message>
<xml_diff>
--- a/data/meta_model/meta_model_R_copy1.xlsx
+++ b/data/meta_model/meta_model_R_copy1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d378ff900cd0a488/Wageningen/Master thesis/R Studio/msc_beeke/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d378ff900cd0a488/Wageningen/Master thesis/R Studio/msc_beeke/data/meta_model/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="8_{E35EF706-6D1C-45D8-8A81-D8A6EFAF874F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4BF5A547-4A50-4E5A-9EA2-2C854C6B1E60}"/>
+  <xr:revisionPtr revIDLastSave="10" documentId="8_{E35EF706-6D1C-45D8-8A81-D8A6EFAF874F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{605FE814-50E4-40CF-9583-49F377A38EB2}"/>
   <bookViews>
-    <workbookView xWindow="32850" yWindow="-15870" windowWidth="25440" windowHeight="15270" firstSheet="2" activeTab="3" xr2:uid="{23E2EBDD-BBB4-413F-B5F8-622405BB80ED}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" activeTab="3" xr2:uid="{23E2EBDD-BBB4-413F-B5F8-622405BB80ED}"/>
   </bookViews>
   <sheets>
     <sheet name="references" sheetId="2" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9030" uniqueCount="376">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8927" uniqueCount="371">
   <si>
     <t>paper_ID</t>
   </si>
@@ -1970,18 +1970,6 @@
     <t>N pool</t>
   </si>
   <si>
-    <t>&gt;6.5</t>
-  </si>
-  <si>
-    <t>&lt;6.5</t>
-  </si>
-  <si>
-    <t>&lt;30%</t>
-  </si>
-  <si>
-    <t>&gt;30%</t>
-  </si>
-  <si>
     <r>
       <t>&lt;10 g kg</t>
     </r>
@@ -2080,9 +2068,6 @@
   </si>
   <si>
     <t>30-40 %</t>
-  </si>
-  <si>
-    <t>*** Mel22 uses a fertilized control and therefore has a different approach the the other papers</t>
   </si>
   <si>
     <t>*** ES for bulk density are negative</t>
@@ -2233,7 +2218,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -2260,7 +2245,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Link" xfId="1" builtinId="8"/>
@@ -2280,9 +2264,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 – 2022-Design">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 – 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2320,7 +2304,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 – 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -2426,7 +2410,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 – 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2568,7 +2552,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2682,34 +2666,18 @@
     <sheetView zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="50" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="H1" sqref="H1"/>
-      <selection pane="bottomLeft" activeCell="Q451" sqref="Q451"/>
+      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="6.3984375" customWidth="1"/>
-    <col min="2" max="2" width="4" customWidth="1"/>
-    <col min="3" max="3" width="10.1328125" customWidth="1"/>
-    <col min="4" max="4" width="5.19921875" customWidth="1"/>
-    <col min="5" max="5" width="4.6640625" customWidth="1"/>
-    <col min="6" max="6" width="10.06640625" customWidth="1"/>
-    <col min="7" max="7" width="11.53125" customWidth="1"/>
-    <col min="8" max="8" width="4.06640625" customWidth="1"/>
-    <col min="9" max="9" width="6.53125" customWidth="1"/>
-    <col min="10" max="10" width="9.796875" customWidth="1"/>
-    <col min="11" max="11" width="12.86328125" customWidth="1"/>
-    <col min="12" max="12" width="4.06640625" customWidth="1"/>
-    <col min="13" max="13" width="7.6640625" customWidth="1"/>
-    <col min="14" max="14" width="4.19921875" customWidth="1"/>
-    <col min="15" max="15" width="14.3984375" customWidth="1"/>
-    <col min="16" max="17" width="4.59765625" customWidth="1"/>
-    <col min="18" max="18" width="4" customWidth="1"/>
-    <col min="19" max="19" width="4.59765625" customWidth="1"/>
-    <col min="20" max="20" width="7.46484375" style="2" customWidth="1"/>
-    <col min="21" max="21" width="8" customWidth="1"/>
-    <col min="22" max="22" width="5.06640625" customWidth="1"/>
-    <col min="24" max="24" width="13.46484375" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="5.06640625" customWidth="1"/>
+    <col min="1" max="1" width="7.73046875" customWidth="1"/>
+    <col min="2" max="2" width="12.86328125" customWidth="1"/>
+    <col min="3" max="3" width="7.9296875" customWidth="1"/>
+    <col min="4" max="4" width="11.86328125" customWidth="1"/>
+    <col min="5" max="19" width="12.86328125" customWidth="1"/>
+    <col min="20" max="20" width="12.86328125" style="2" customWidth="1"/>
+    <col min="21" max="26" width="12.86328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:28" x14ac:dyDescent="0.45">
@@ -33183,10 +33151,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D463793D-A6D7-4CC6-BF64-63A98439A959}">
-  <dimension ref="A1:L23"/>
+  <dimension ref="A1:L17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD5"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -33639,32 +33607,6 @@
         <v>27</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A23" t="s">
-        <v>115</v>
-      </c>
-      <c r="B23" t="s">
-        <v>12</v>
-      </c>
-      <c r="C23" t="s">
-        <v>117</v>
-      </c>
-      <c r="E23" t="s">
-        <v>17</v>
-      </c>
-      <c r="F23" t="s">
-        <v>296</v>
-      </c>
-      <c r="J23" s="5">
-        <v>10</v>
-      </c>
-      <c r="K23">
-        <v>2.3991370545788135</v>
-      </c>
-      <c r="L23">
-        <v>40</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
@@ -33672,11 +33614,11 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0108F44-9AB1-43D9-B41B-7BC1ED64F125}">
-  <dimension ref="A1:N526"/>
+  <dimension ref="A1:N501"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O5" sqref="O5"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A495" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B505" sqref="B505"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -33705,22 +33647,22 @@
         <v>261</v>
       </c>
       <c r="D1" t="s">
-        <v>374</v>
+        <v>369</v>
       </c>
       <c r="E1" t="s">
         <v>252</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>372</v>
+        <v>367</v>
       </c>
       <c r="G1" t="s">
-        <v>375</v>
+        <v>370</v>
       </c>
       <c r="H1" t="s">
         <v>253</v>
       </c>
       <c r="I1" t="s">
-        <v>373</v>
+        <v>368</v>
       </c>
       <c r="J1" t="s">
         <v>254</v>
@@ -40783,7 +40725,7 @@
         <v>49</v>
       </c>
       <c r="N226" s="1" t="s">
-        <v>371</v>
+        <v>366</v>
       </c>
     </row>
     <row r="227" spans="1:14" ht="15.75" x14ac:dyDescent="0.45">
@@ -40931,7 +40873,7 @@
         <v>43</v>
       </c>
       <c r="J231" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="K231" s="5">
         <v>-6.8686868686868596</v>
@@ -40966,7 +40908,7 @@
         <v>43</v>
       </c>
       <c r="J232" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="K232" s="5">
         <v>-9.3602693602693599</v>
@@ -41001,7 +40943,7 @@
         <v>43</v>
       </c>
       <c r="J233" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="K233" s="5">
         <v>-10.639730639730599</v>
@@ -41106,7 +41048,7 @@
         <v>44</v>
       </c>
       <c r="J236" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="K236" s="5">
         <v>-10.909090909090899</v>
@@ -41141,7 +41083,7 @@
         <v>44</v>
       </c>
       <c r="J237" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="K237" s="5">
         <v>-5.7912457912457898</v>
@@ -41176,7 +41118,7 @@
         <v>44</v>
       </c>
       <c r="J238" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="K238" s="5">
         <v>-5.7912457912457898</v>
@@ -41281,7 +41223,7 @@
         <v>44</v>
       </c>
       <c r="J241" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="K241" s="5">
         <v>-4.7811447811447803</v>
@@ -41316,7 +41258,7 @@
         <v>44</v>
       </c>
       <c r="J242" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="K242" s="5">
         <v>-4.7811447811447803</v>
@@ -41351,7 +41293,7 @@
         <v>45</v>
       </c>
       <c r="J243" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="K243" s="5">
         <v>-12.7272727272727</v>
@@ -41456,7 +41398,7 @@
         <v>45</v>
       </c>
       <c r="J246" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="K246" s="5">
         <v>-9.6969696969696901</v>
@@ -41491,7 +41433,7 @@
         <v>45</v>
       </c>
       <c r="J247" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="K247" s="5">
         <v>-6.2626262626262603</v>
@@ -41526,7 +41468,7 @@
         <v>45</v>
       </c>
       <c r="J248" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="K248" s="5">
         <v>-6.2626262626262603</v>
@@ -41584,7 +41526,7 @@
         <v>145</v>
       </c>
       <c r="E250" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="F250" t="s">
         <v>151</v>
@@ -41596,7 +41538,7 @@
         <v>43</v>
       </c>
       <c r="J250" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="K250" s="5">
         <v>-11.1784511784511</v>
@@ -41619,7 +41561,7 @@
         <v>145</v>
       </c>
       <c r="E251" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="F251" t="s">
         <v>148</v>
@@ -41631,7 +41573,7 @@
         <v>43</v>
       </c>
       <c r="J251" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="K251" s="5">
         <v>-11.8518518518518</v>
@@ -41654,7 +41596,7 @@
         <v>145</v>
       </c>
       <c r="E252" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="F252" t="s">
         <v>149</v>
@@ -41689,7 +41631,7 @@
         <v>145</v>
       </c>
       <c r="E253" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="F253" t="s">
         <v>150</v>
@@ -41701,7 +41643,7 @@
         <v>43</v>
       </c>
       <c r="J253" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="K253" s="5">
         <v>-6.5993265993266004</v>
@@ -41724,7 +41666,7 @@
         <v>145</v>
       </c>
       <c r="E254" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="F254" t="s">
         <v>151</v>
@@ -41736,7 +41678,7 @@
         <v>44</v>
       </c>
       <c r="J254" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="K254" s="5">
         <v>-8.4175084175084098</v>
@@ -41759,7 +41701,7 @@
         <v>145</v>
       </c>
       <c r="E255" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="F255" t="s">
         <v>148</v>
@@ -41794,7 +41736,7 @@
         <v>145</v>
       </c>
       <c r="E256" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="F256" t="s">
         <v>149</v>
@@ -41806,7 +41748,7 @@
         <v>44</v>
       </c>
       <c r="J256" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="K256" s="5">
         <v>-6.12794612794612</v>
@@ -41829,7 +41771,7 @@
         <v>145</v>
       </c>
       <c r="E257" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="F257" t="s">
         <v>150</v>
@@ -41841,7 +41783,7 @@
         <v>44</v>
       </c>
       <c r="J257" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="K257" s="5">
         <v>-7.4747474747474696</v>
@@ -41864,7 +41806,7 @@
         <v>145</v>
       </c>
       <c r="E258" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="F258" t="s">
         <v>151</v>
@@ -41899,7 +41841,7 @@
         <v>145</v>
       </c>
       <c r="E259" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="F259" t="s">
         <v>148</v>
@@ -41911,7 +41853,7 @@
         <v>45</v>
       </c>
       <c r="J259" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="K259" s="5">
         <v>-9.96632996632996</v>
@@ -41934,7 +41876,7 @@
         <v>145</v>
       </c>
       <c r="E260" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="F260" t="s">
         <v>149</v>
@@ -41946,7 +41888,7 @@
         <v>45</v>
       </c>
       <c r="J260" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="K260" s="5">
         <v>-3.7037037037037002</v>
@@ -41969,7 +41911,7 @@
         <v>145</v>
       </c>
       <c r="E261" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="F261" t="s">
         <v>150</v>
@@ -42051,7 +41993,7 @@
         <v>43</v>
       </c>
       <c r="J263" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="K263" s="5">
         <v>-7.4747474747474696</v>
@@ -42086,7 +42028,7 @@
         <v>43</v>
       </c>
       <c r="J264" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="K264" s="5">
         <v>-11.649831649831601</v>
@@ -42191,7 +42133,7 @@
         <v>44</v>
       </c>
       <c r="J267" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="K267" s="5">
         <v>-7.87878787878787</v>
@@ -42226,7 +42168,7 @@
         <v>45</v>
       </c>
       <c r="J268" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="K268" s="5">
         <v>-5.9932659932659904</v>
@@ -42331,7 +42273,7 @@
         <v>43</v>
       </c>
       <c r="J271" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="K271" s="5">
         <v>-5.0961538461538396</v>
@@ -42366,7 +42308,7 @@
         <v>43</v>
       </c>
       <c r="J272" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="K272" s="5">
         <v>-3.9423076923076898</v>
@@ -42471,7 +42413,7 @@
         <v>45</v>
       </c>
       <c r="J275" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="K275" s="5">
         <v>-12.019230769230701</v>
@@ -42491,7 +42433,7 @@
         <v>136</v>
       </c>
       <c r="D276" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
       <c r="E276" t="s">
         <v>34</v>
@@ -42506,7 +42448,7 @@
         <v>43</v>
       </c>
       <c r="J276" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="K276" s="5">
         <v>-7.6923076923076898</v>
@@ -42526,7 +42468,7 @@
         <v>136</v>
       </c>
       <c r="D277" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
       <c r="E277" t="s">
         <v>33</v>
@@ -42561,7 +42503,7 @@
         <v>136</v>
       </c>
       <c r="D278" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
       <c r="E278" t="s">
         <v>35</v>
@@ -42596,7 +42538,7 @@
         <v>136</v>
       </c>
       <c r="D279" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
       <c r="E279" t="s">
         <v>36</v>
@@ -42611,7 +42553,7 @@
         <v>43</v>
       </c>
       <c r="J279" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="K279" s="5">
         <v>-7.1153846153846203</v>
@@ -42631,7 +42573,7 @@
         <v>136</v>
       </c>
       <c r="D280" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
       <c r="E280" t="s">
         <v>35</v>
@@ -42646,7 +42588,7 @@
         <v>44</v>
       </c>
       <c r="J280" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="K280" s="5">
         <v>-3.9423076923076898</v>
@@ -42666,7 +42608,7 @@
         <v>136</v>
       </c>
       <c r="D281" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
       <c r="E281" t="s">
         <v>34</v>
@@ -42701,7 +42643,7 @@
         <v>136</v>
       </c>
       <c r="D282" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
       <c r="E282" t="s">
         <v>35</v>
@@ -42736,7 +42678,7 @@
         <v>136</v>
       </c>
       <c r="D283" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
       <c r="E283" t="s">
         <v>36</v>
@@ -42751,7 +42693,7 @@
         <v>45</v>
       </c>
       <c r="J283" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="K283" s="5">
         <v>-16.923076923076898</v>
@@ -42786,7 +42728,7 @@
         <v>43</v>
       </c>
       <c r="J284" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="K284" s="5">
         <v>-15.769230769230701</v>
@@ -42891,7 +42833,7 @@
         <v>43</v>
       </c>
       <c r="J287" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="K287" s="5">
         <v>-7.6923076923076898</v>
@@ -42926,7 +42868,7 @@
         <v>44</v>
       </c>
       <c r="J288" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="K288" s="5">
         <v>-7.9807692307692299</v>
@@ -43031,7 +42973,7 @@
         <v>45</v>
       </c>
       <c r="J291" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="K291" s="5">
         <v>-9.7115384615384599</v>
@@ -43066,7 +43008,7 @@
         <v>45</v>
       </c>
       <c r="J292" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="K292" s="5">
         <v>-4.8076923076923102</v>
@@ -43171,7 +43113,7 @@
         <v>43</v>
       </c>
       <c r="J295" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="K295" s="5">
         <v>-10.288461538461499</v>
@@ -43206,7 +43148,7 @@
         <v>43</v>
       </c>
       <c r="J296" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="K296" s="5">
         <v>-14.615384615384601</v>
@@ -43311,7 +43253,7 @@
         <v>44</v>
       </c>
       <c r="J299" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="K299" s="5">
         <v>-7.4038461538461497</v>
@@ -43346,7 +43288,7 @@
         <v>44</v>
       </c>
       <c r="J300" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="K300" s="5">
         <v>-8.5576923076923102</v>
@@ -43451,7 +43393,7 @@
         <v>45</v>
       </c>
       <c r="J303" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="K303" s="5">
         <v>-8.8461538461538503</v>
@@ -43486,7 +43428,7 @@
         <v>45</v>
       </c>
       <c r="J304" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="K304" s="5">
         <v>-6.8269230769230802</v>
@@ -43592,7 +43534,7 @@
       </c>
       <c r="I307" s="8"/>
       <c r="J307" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="K307" s="5">
         <v>-12.307692307692299</v>
@@ -43628,7 +43570,7 @@
       </c>
       <c r="I308" s="8"/>
       <c r="J308" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="K308" s="5">
         <v>-9.4230769230769198</v>
@@ -43736,7 +43678,7 @@
       </c>
       <c r="I311" s="8"/>
       <c r="J311" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="K311" s="5">
         <v>-12.019230769230701</v>
@@ -43772,7 +43714,7 @@
       </c>
       <c r="I312" s="8"/>
       <c r="J312" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="K312" s="5">
         <v>-7.9807692307692299</v>
@@ -43880,7 +43822,7 @@
       </c>
       <c r="I315" s="8"/>
       <c r="J315" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="K315" s="5">
         <v>-9.1346153846153797</v>
@@ -43916,7 +43858,7 @@
       </c>
       <c r="I316" s="8"/>
       <c r="J316" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="K316" s="5">
         <v>-19.807692307692299</v>
@@ -44021,7 +43963,7 @@
         <v>43</v>
       </c>
       <c r="J319" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="K319" s="5">
         <v>-6.5384615384615401</v>
@@ -44056,7 +43998,7 @@
         <v>43</v>
       </c>
       <c r="J320" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="K320" s="5">
         <v>-6.8269230769230802</v>
@@ -44161,7 +44103,7 @@
         <v>44</v>
       </c>
       <c r="J323" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="K323" s="5">
         <v>-8.2692307692307701</v>
@@ -44196,7 +44138,7 @@
         <v>44</v>
       </c>
       <c r="J324" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="K324" s="5">
         <v>-8.2692307692307701</v>
@@ -44301,7 +44243,7 @@
         <v>45</v>
       </c>
       <c r="J327" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="K327" s="5">
         <v>-8.2692307692307701</v>
@@ -44328,7 +44270,7 @@
       </c>
       <c r="F328"/>
       <c r="J328" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="K328" s="5">
         <v>12.3</v>
@@ -44355,7 +44297,7 @@
       </c>
       <c r="F329"/>
       <c r="J329" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="K329" s="5">
         <v>7.2</v>
@@ -44382,7 +44324,7 @@
       </c>
       <c r="F330"/>
       <c r="J330" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="K330" s="5">
         <v>5.5</v>
@@ -44417,7 +44359,7 @@
         <v>43</v>
       </c>
       <c r="J331" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="K331" s="5">
         <v>15.156950672645699</v>
@@ -44452,7 +44394,7 @@
         <v>43</v>
       </c>
       <c r="J332" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="K332" s="5">
         <v>5.65022421524663</v>
@@ -44487,7 +44429,7 @@
         <v>43</v>
       </c>
       <c r="J333" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="K333" s="5">
         <v>5.65022421524663</v>
@@ -44522,7 +44464,7 @@
         <v>43</v>
       </c>
       <c r="J334" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="K334" s="5">
         <v>-21.076233183856498</v>
@@ -44557,7 +44499,7 @@
         <v>43</v>
       </c>
       <c r="J335" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="K335" s="5">
         <v>-21.076233183856498</v>
@@ -44592,7 +44534,7 @@
         <v>43</v>
       </c>
       <c r="J336" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="K336" s="5">
         <v>-21.076233183856498</v>
@@ -44627,7 +44569,7 @@
         <v>44</v>
       </c>
       <c r="J337" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="K337" s="5">
         <v>12.825112107623299</v>
@@ -44662,7 +44604,7 @@
         <v>44</v>
       </c>
       <c r="J338" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="K338" s="5">
         <v>8.3408071748878907</v>
@@ -44697,7 +44639,7 @@
         <v>44</v>
       </c>
       <c r="J339" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="K339" s="5">
         <v>6.18834080717488</v>
@@ -44732,7 +44674,7 @@
         <v>44</v>
       </c>
       <c r="J340" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="K340" s="5">
         <v>3.3183856502242102</v>
@@ -44767,7 +44709,7 @@
         <v>45</v>
       </c>
       <c r="J341" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="K341" s="5">
         <v>8.6995515695067205</v>
@@ -44802,7 +44744,7 @@
         <v>45</v>
       </c>
       <c r="J342" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="K342" s="5">
         <v>7.26457399103138</v>
@@ -44837,7 +44779,7 @@
         <v>45</v>
       </c>
       <c r="J343" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="K343" s="5">
         <v>4.57399103139013</v>
@@ -44872,7 +44814,7 @@
         <v>45</v>
       </c>
       <c r="J344" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="K344" s="5">
         <v>-2.9596412556053799</v>
@@ -44907,7 +44849,7 @@
         <v>45</v>
       </c>
       <c r="J345" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="K345" s="5">
         <v>-2.9596412556053799</v>
@@ -44942,7 +44884,7 @@
         <v>45</v>
       </c>
       <c r="J346" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="K346" s="5">
         <v>-2.9596412556053799</v>
@@ -44977,7 +44919,7 @@
         <v>43</v>
       </c>
       <c r="J347" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="K347" s="5">
         <v>8.6995515695067205</v>
@@ -45012,7 +44954,7 @@
         <v>43</v>
       </c>
       <c r="J348" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="K348" s="5">
         <v>18.923766816143399</v>
@@ -45047,7 +44989,7 @@
         <v>43</v>
       </c>
       <c r="J349" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="K349" s="5">
         <v>29.686098654708498</v>
@@ -45082,7 +45024,7 @@
         <v>43</v>
       </c>
       <c r="J350" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="K350" s="5">
         <v>12.6457399103139</v>
@@ -45117,7 +45059,7 @@
         <v>44</v>
       </c>
       <c r="J351" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="K351" s="5">
         <v>10.134529147982001</v>
@@ -45152,7 +45094,7 @@
         <v>45</v>
       </c>
       <c r="J352" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="K352" s="5">
         <v>2.2421524663677102</v>
@@ -45187,7 +45129,7 @@
         <v>43</v>
       </c>
       <c r="J353" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="K353" s="5">
         <v>1.1659192825111999</v>
@@ -45222,7 +45164,7 @@
         <v>43</v>
       </c>
       <c r="J354" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="K354" s="5">
         <v>3.8565022421524602</v>
@@ -45257,7 +45199,7 @@
         <v>43</v>
       </c>
       <c r="J355" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="K355" s="5">
         <v>16.412556053811599</v>
@@ -45292,7 +45234,7 @@
         <v>44</v>
       </c>
       <c r="J356" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="K356" s="5">
         <v>13.901345291479799</v>
@@ -45327,7 +45269,7 @@
         <v>44</v>
       </c>
       <c r="J357" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="K357" s="5">
         <v>3.4977578475336299</v>
@@ -45362,7 +45304,7 @@
         <v>44</v>
       </c>
       <c r="J358" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="K358" s="5">
         <v>10.134529147982001</v>
@@ -45397,7 +45339,7 @@
         <v>45</v>
       </c>
       <c r="J359" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="K359" s="5">
         <v>7.4439461883408002</v>
@@ -45432,7 +45374,7 @@
         <v>45</v>
       </c>
       <c r="J360" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="K360" s="5">
         <v>2.7802690582959602</v>
@@ -45467,7 +45409,7 @@
         <v>43</v>
       </c>
       <c r="J361" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="K361" s="5">
         <v>4.2222222222222197</v>
@@ -45502,7 +45444,7 @@
         <v>43</v>
       </c>
       <c r="J362" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="K362" s="5">
         <v>15.422222222222199</v>
@@ -45537,7 +45479,7 @@
         <v>44</v>
       </c>
       <c r="J363" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="K363" s="5">
         <v>6</v>
@@ -45560,10 +45502,10 @@
         <v>53</v>
       </c>
       <c r="E364" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="F364" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
       <c r="G364" t="s">
         <v>42</v>
@@ -45572,7 +45514,7 @@
         <v>44</v>
       </c>
       <c r="J364" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="K364" s="5">
         <v>9.0222222222222204</v>
@@ -45607,7 +45549,7 @@
         <v>44</v>
       </c>
       <c r="J365" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="K365" s="5">
         <v>7.7777777777777697</v>
@@ -45630,7 +45572,7 @@
         <v>53</v>
       </c>
       <c r="E366" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="F366" t="s">
         <v>155</v>
@@ -45642,7 +45584,7 @@
         <v>45</v>
       </c>
       <c r="J366" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="K366" s="5">
         <v>2.2666666666666599</v>
@@ -45662,7 +45604,7 @@
         <v>137</v>
       </c>
       <c r="D367" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
       <c r="E367" t="s">
         <v>33</v>
@@ -45677,7 +45619,7 @@
         <v>43</v>
       </c>
       <c r="J367" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="K367" s="5">
         <v>25.733333333333299</v>
@@ -45697,7 +45639,7 @@
         <v>137</v>
       </c>
       <c r="D368" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
       <c r="E368" t="s">
         <v>35</v>
@@ -45712,7 +45654,7 @@
         <v>43</v>
       </c>
       <c r="J368" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="K368" s="5">
         <v>12.9333333333333</v>
@@ -45732,7 +45674,7 @@
         <v>137</v>
       </c>
       <c r="D369" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
       <c r="E369" t="s">
         <v>36</v>
@@ -45747,7 +45689,7 @@
         <v>43</v>
       </c>
       <c r="J369" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="K369" s="5">
         <v>23.955555555555499</v>
@@ -45767,7 +45709,7 @@
         <v>137</v>
       </c>
       <c r="D370" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
       <c r="E370" t="s">
         <v>34</v>
@@ -45782,7 +45724,7 @@
         <v>45</v>
       </c>
       <c r="J370" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="K370" s="5">
         <v>-3.24444444444444</v>
@@ -45802,7 +45744,7 @@
         <v>137</v>
       </c>
       <c r="D371" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
       <c r="E371" t="s">
         <v>35</v>
@@ -45817,7 +45759,7 @@
         <v>45</v>
       </c>
       <c r="J371" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="K371" s="5">
         <v>5.4666666666666597</v>
@@ -45852,7 +45794,7 @@
         <v>43</v>
       </c>
       <c r="J372" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="K372" s="5">
         <v>5.4666666666666597</v>
@@ -45887,7 +45829,7 @@
         <v>43</v>
       </c>
       <c r="J373" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="K373" s="5">
         <v>10.9777777777777</v>
@@ -45922,7 +45864,7 @@
         <v>43</v>
       </c>
       <c r="J374" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="K374" s="5">
         <v>12.9333333333333</v>
@@ -45957,7 +45899,7 @@
         <v>44</v>
       </c>
       <c r="J375" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="K375" s="5">
         <v>1.0222222222222199</v>
@@ -45992,7 +45934,7 @@
         <v>45</v>
       </c>
       <c r="J376" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="K376" s="5">
         <v>2.2666666666666599</v>
@@ -46027,7 +45969,7 @@
         <v>45</v>
       </c>
       <c r="J377" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="K377" s="5">
         <v>8.1333333333333293</v>
@@ -46062,7 +46004,7 @@
         <v>43</v>
       </c>
       <c r="J378" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="K378" s="5">
         <v>13.1111111111111</v>
@@ -46097,7 +46039,7 @@
         <v>43</v>
       </c>
       <c r="J379" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="K379" s="5">
         <v>19.688888888888801</v>
@@ -46132,7 +46074,7 @@
         <v>43</v>
       </c>
       <c r="J380" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="K380" s="5">
         <v>5.8222222222222202</v>
@@ -46167,7 +46109,7 @@
         <v>43</v>
       </c>
       <c r="J381" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="K381" s="5">
         <v>21.288888888888799</v>
@@ -46202,7 +46144,7 @@
         <v>44</v>
       </c>
       <c r="J382" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="K382" s="5">
         <v>-2.3555555555555499</v>
@@ -46237,7 +46179,7 @@
         <v>44</v>
       </c>
       <c r="J383" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="K383" s="5">
         <v>9.7333333333333307</v>
@@ -46272,7 +46214,7 @@
         <v>44</v>
       </c>
       <c r="J384" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="K384" s="5">
         <v>5.1111111111111098</v>
@@ -46307,7 +46249,7 @@
         <v>45</v>
       </c>
       <c r="J385" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="K385" s="5">
         <v>2.4444444444444402</v>
@@ -46342,7 +46284,7 @@
         <v>45</v>
       </c>
       <c r="J386" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="K386" s="5">
         <v>6.5333333333333297</v>
@@ -46378,7 +46320,7 @@
       </c>
       <c r="I387" s="8"/>
       <c r="J387" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="K387" s="5">
         <v>12.7555555555555</v>
@@ -46414,7 +46356,7 @@
       </c>
       <c r="I388" s="8"/>
       <c r="J388" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="K388" s="5">
         <v>22.711111111111101</v>
@@ -46450,7 +46392,7 @@
       </c>
       <c r="I389" s="8"/>
       <c r="J389" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="K389" s="5">
         <v>29.288888888888799</v>
@@ -46486,7 +46428,7 @@
       </c>
       <c r="I390" s="8"/>
       <c r="J390" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="K390" s="5">
         <v>9.0222222222222204</v>
@@ -46522,7 +46464,7 @@
       </c>
       <c r="I391" s="8"/>
       <c r="J391" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="K391" s="5">
         <v>3.68888888888889</v>
@@ -46558,7 +46500,7 @@
       </c>
       <c r="I392" s="8"/>
       <c r="J392" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="K392" s="5">
         <v>-3.24444444444444</v>
@@ -46593,7 +46535,7 @@
         <v>43</v>
       </c>
       <c r="J393" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="K393" s="5">
         <v>4.2222222222222197</v>
@@ -46628,7 +46570,7 @@
         <v>43</v>
       </c>
       <c r="J394" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="K394" s="5">
         <v>29.822222222222202</v>
@@ -46663,7 +46605,7 @@
         <v>43</v>
       </c>
       <c r="J395" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="K395" s="5">
         <v>10.9777777777777</v>
@@ -46698,7 +46640,7 @@
         <v>43</v>
       </c>
       <c r="J396" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="K396" s="5">
         <v>13.6444444444444</v>
@@ -46733,7 +46675,7 @@
         <v>44</v>
       </c>
       <c r="J397" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="K397" s="5">
         <v>8.8444444444444397</v>
@@ -46768,7 +46710,7 @@
         <v>44</v>
       </c>
       <c r="J398" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="K398" s="5">
         <v>4.7555555555555502</v>
@@ -46803,7 +46745,7 @@
         <v>44</v>
       </c>
       <c r="J399" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="K399" s="5">
         <v>7.6</v>
@@ -46838,7 +46780,7 @@
         <v>44</v>
       </c>
       <c r="J400" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="K400" s="5">
         <v>6</v>
@@ -46873,7 +46815,7 @@
         <v>45</v>
       </c>
       <c r="J401" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="K401" s="5">
         <v>9.0222222222222204</v>
@@ -46908,7 +46850,7 @@
         <v>45</v>
       </c>
       <c r="J402" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="K402" s="5">
         <v>4.0444444444444398</v>
@@ -46943,7 +46885,7 @@
         <v>45</v>
       </c>
       <c r="J403" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="K403" s="5">
         <v>2.2666666666666599</v>
@@ -47539,7 +47481,7 @@
         <v>36</v>
       </c>
       <c r="F425" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="K425" s="8">
         <v>10.6199460916442</v>
@@ -47568,7 +47510,7 @@
         <v>35</v>
       </c>
       <c r="F426" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="K426" s="8">
         <v>10.6199460916442</v>
@@ -47626,7 +47568,7 @@
         <v>33</v>
       </c>
       <c r="F428" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="K428" s="8">
         <v>9.8113207547169807</v>
@@ -47655,7 +47597,7 @@
         <v>34</v>
       </c>
       <c r="F429" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="K429" s="8">
         <v>9.8113207547169807</v>
@@ -48743,7 +48685,7 @@
         <v>91</v>
       </c>
       <c r="F470" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="K470" s="5">
         <v>14.833702882483299</v>
@@ -48769,7 +48711,7 @@
         <v>91</v>
       </c>
       <c r="F471" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
       <c r="K471" s="5">
         <v>16.829268292682901</v>
@@ -48795,7 +48737,7 @@
         <v>91</v>
       </c>
       <c r="F472" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="K472" s="5">
         <v>13.237250554323699</v>
@@ -48821,7 +48763,7 @@
         <v>91</v>
       </c>
       <c r="F473" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="K473" s="5">
         <v>7.9157427937915701</v>
@@ -48847,7 +48789,7 @@
         <v>91</v>
       </c>
       <c r="F474" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="K474" s="5">
         <v>6.1197339246119702</v>
@@ -49306,7 +49248,7 @@
         <v>91</v>
       </c>
       <c r="F492" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="K492" s="5">
         <v>45.232815964523198</v>
@@ -49332,7 +49274,7 @@
         <v>91</v>
       </c>
       <c r="F493" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
       <c r="K493" s="5">
         <v>45.232815964523198</v>
@@ -49358,7 +49300,7 @@
         <v>91</v>
       </c>
       <c r="F494" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="K494" s="5">
         <v>34.146341463414601</v>
@@ -49384,7 +49326,7 @@
         <v>91</v>
       </c>
       <c r="F495" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="K495" s="5">
         <v>26.829268292682901</v>
@@ -49410,7 +49352,7 @@
         <v>91</v>
       </c>
       <c r="F496" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="K496" s="5">
         <v>12.6385809312638</v>
@@ -49550,494 +49492,6 @@
       </c>
       <c r="M501" s="8">
         <v>125</v>
-      </c>
-    </row>
-    <row r="508" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A508" s="1" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="510" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A510" s="7" t="s">
-        <v>115</v>
-      </c>
-      <c r="B510" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="C510" s="7" t="s">
-        <v>117</v>
-      </c>
-      <c r="D510" s="7" t="s">
-        <v>267</v>
-      </c>
-      <c r="E510" s="7" t="s">
-        <v>131</v>
-      </c>
-      <c r="F510" s="20"/>
-      <c r="K510" s="18">
-        <v>10</v>
-      </c>
-      <c r="L510" s="7">
-        <v>4.0915515659483557</v>
-      </c>
-      <c r="M510" s="7">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="511" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A511" s="7" t="s">
-        <v>115</v>
-      </c>
-      <c r="B511" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="C511" s="7" t="s">
-        <v>117</v>
-      </c>
-      <c r="D511" s="7" t="s">
-        <v>267</v>
-      </c>
-      <c r="E511" s="7" t="s">
-        <v>132</v>
-      </c>
-      <c r="F511" s="20"/>
-      <c r="K511" s="18">
-        <v>7</v>
-      </c>
-      <c r="L511" s="7">
-        <v>3.1058595977880632</v>
-      </c>
-      <c r="M511" s="7">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="512" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A512" s="7" t="s">
-        <v>115</v>
-      </c>
-      <c r="B512" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="C512" s="7" t="s">
-        <v>117</v>
-      </c>
-      <c r="D512" s="7" t="s">
-        <v>118</v>
-      </c>
-      <c r="E512" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="F512" s="7" t="s">
-        <v>349</v>
-      </c>
-      <c r="K512" s="18">
-        <v>10</v>
-      </c>
-      <c r="L512" s="7">
-        <v>3.8869739876509355</v>
-      </c>
-      <c r="M512" s="7">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="513" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A513" s="7" t="s">
-        <v>115</v>
-      </c>
-      <c r="B513" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="C513" s="7" t="s">
-        <v>117</v>
-      </c>
-      <c r="D513" s="7" t="s">
-        <v>118</v>
-      </c>
-      <c r="E513" s="7" t="s">
-        <v>90</v>
-      </c>
-      <c r="F513" s="7" t="s">
-        <v>349</v>
-      </c>
-      <c r="K513" s="18">
-        <v>10</v>
-      </c>
-      <c r="L513" s="7">
-        <v>3.8869739876509355</v>
-      </c>
-      <c r="M513" s="7">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="514" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A514" s="7" t="s">
-        <v>115</v>
-      </c>
-      <c r="B514" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="C514" s="7" t="s">
-        <v>117</v>
-      </c>
-      <c r="D514" s="7" t="s">
-        <v>118</v>
-      </c>
-      <c r="E514" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="F514" s="7" t="s">
-        <v>349</v>
-      </c>
-      <c r="K514" s="18">
-        <v>10</v>
-      </c>
-      <c r="L514" s="7">
-        <v>3.8869739876509355</v>
-      </c>
-      <c r="M514" s="7">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="515" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A515" s="7" t="s">
-        <v>115</v>
-      </c>
-      <c r="B515" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="C515" s="7" t="s">
-        <v>117</v>
-      </c>
-      <c r="D515" s="7" t="s">
-        <v>118</v>
-      </c>
-      <c r="E515" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="F515" s="7" t="s">
-        <v>350</v>
-      </c>
-      <c r="K515" s="18">
-        <v>10</v>
-      </c>
-      <c r="L515" s="7">
-        <v>3.2732412527586967</v>
-      </c>
-      <c r="M515" s="7">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="516" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A516" s="7" t="s">
-        <v>115</v>
-      </c>
-      <c r="B516" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="C516" s="7" t="s">
-        <v>117</v>
-      </c>
-      <c r="D516" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="E516" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="F516" s="20"/>
-      <c r="K516" s="18">
-        <v>8</v>
-      </c>
-      <c r="L516" s="7">
-        <v>2.8826840578272548</v>
-      </c>
-      <c r="M516" s="7">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="517" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A517" s="7" t="s">
-        <v>115</v>
-      </c>
-      <c r="B517" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="C517" s="7" t="s">
-        <v>117</v>
-      </c>
-      <c r="D517" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="E517" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="F517" s="20"/>
-      <c r="K517" s="18">
-        <v>11</v>
-      </c>
-      <c r="L517" s="7">
-        <v>3.5522106777097195</v>
-      </c>
-      <c r="M517" s="7">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="518" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A518" s="7" t="s">
-        <v>115</v>
-      </c>
-      <c r="B518" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="C518" s="7" t="s">
-        <v>117</v>
-      </c>
-      <c r="D518" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="E518" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="F518" s="20"/>
-      <c r="K518" s="18">
-        <v>6</v>
-      </c>
-      <c r="L518" s="7">
-        <v>4.3333250675725736</v>
-      </c>
-      <c r="M518" s="7">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="519" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A519" s="7" t="s">
-        <v>115</v>
-      </c>
-      <c r="B519" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="C519" s="7" t="s">
-        <v>117</v>
-      </c>
-      <c r="D519" s="7" t="s">
-        <v>262</v>
-      </c>
-      <c r="E519" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="F519" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="K519" s="18">
-        <v>17</v>
-      </c>
-      <c r="L519" s="7">
-        <v>3.3290351377489031</v>
-      </c>
-      <c r="M519" s="7">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="520" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A520" s="7" t="s">
-        <v>115</v>
-      </c>
-      <c r="B520" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="C520" s="7" t="s">
-        <v>117</v>
-      </c>
-      <c r="D520" s="7" t="s">
-        <v>262</v>
-      </c>
-      <c r="E520" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="F520" s="7" t="s">
-        <v>127</v>
-      </c>
-      <c r="K520" s="18">
-        <v>7</v>
-      </c>
-      <c r="L520" s="7">
-        <v>10.080095221563699</v>
-      </c>
-      <c r="M520" s="7">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="521" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A521" s="7" t="s">
-        <v>115</v>
-      </c>
-      <c r="B521" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="C521" s="7" t="s">
-        <v>117</v>
-      </c>
-      <c r="D521" s="7" t="s">
-        <v>262</v>
-      </c>
-      <c r="E521" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="F521" s="7" t="s">
-        <v>125</v>
-      </c>
-      <c r="K521" s="18">
-        <v>3</v>
-      </c>
-      <c r="L521" s="7">
-        <v>3.0686636744612752</v>
-      </c>
-      <c r="M521" s="7">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="522" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A522" s="7" t="s">
-        <v>115</v>
-      </c>
-      <c r="B522" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="C522" s="7" t="s">
-        <v>117</v>
-      </c>
-      <c r="D522" s="7" t="s">
-        <v>164</v>
-      </c>
-      <c r="E522" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="F522" s="7" t="s">
-        <v>351</v>
-      </c>
-      <c r="K522" s="18">
-        <v>5</v>
-      </c>
-      <c r="L522" s="7">
-        <v>2.8454881345004548</v>
-      </c>
-      <c r="M522" s="7">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="523" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A523" s="7" t="s">
-        <v>115</v>
-      </c>
-      <c r="B523" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="C523" s="7" t="s">
-        <v>117</v>
-      </c>
-      <c r="D523" s="7" t="s">
-        <v>164</v>
-      </c>
-      <c r="E523" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="F523" s="7" t="s">
-        <v>352</v>
-      </c>
-      <c r="K523" s="18">
-        <v>17</v>
-      </c>
-      <c r="L523" s="7">
-        <v>3.1244575594515052</v>
-      </c>
-      <c r="M523" s="7">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="524" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A524" s="7" t="s">
-        <v>115</v>
-      </c>
-      <c r="B524" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="C524" s="7" t="s">
-        <v>117</v>
-      </c>
-      <c r="D524" s="7" t="s">
-        <v>164</v>
-      </c>
-      <c r="E524" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="F524" s="7" t="s">
-        <v>352</v>
-      </c>
-      <c r="K524" s="18">
-        <v>17</v>
-      </c>
-      <c r="L524" s="7">
-        <v>3.1244575594515052</v>
-      </c>
-      <c r="M524" s="7">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="525" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A525" s="7" t="s">
-        <v>115</v>
-      </c>
-      <c r="B525" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="C525" s="7" t="s">
-        <v>117</v>
-      </c>
-      <c r="D525" s="7" t="s">
-        <v>164</v>
-      </c>
-      <c r="E525" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="F525" s="7" t="s">
-        <v>352</v>
-      </c>
-      <c r="K525" s="18">
-        <v>17</v>
-      </c>
-      <c r="L525" s="7">
-        <v>3.1244575594515052</v>
-      </c>
-      <c r="M525" s="7">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="526" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A526" s="7" t="s">
-        <v>115</v>
-      </c>
-      <c r="B526" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="C526" s="7" t="s">
-        <v>117</v>
-      </c>
-      <c r="D526" s="7" t="s">
-        <v>164</v>
-      </c>
-      <c r="E526" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="F526" s="7" t="s">
-        <v>352</v>
-      </c>
-      <c r="K526" s="18">
-        <v>17</v>
-      </c>
-      <c r="L526" s="7">
-        <v>3.1244575594515052</v>
-      </c>
-      <c r="M526" s="7">
-        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>